<commit_message>
updated isbn validation,covers, barcode note, form disabled after submit
</commit_message>
<xml_diff>
--- a/selfPublishing data.xlsx
+++ b/selfPublishing data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="494" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="494" uniqueCount="91">
   <si>
     <r>
       <t> </t>
@@ -418,9 +418,6 @@
   </si>
   <si>
     <t>proj_id</t>
-  </si>
-  <si>
-    <t>double</t>
   </si>
   <si>
     <t>template_id</t>
@@ -1910,7 +1907,7 @@
   <dimension ref="A1:M30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+      <selection activeCell="M22" sqref="M22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1923,10 +1920,10 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="E1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -2146,7 +2143,7 @@
         <v>29</v>
       </c>
       <c r="G13" t="s">
-        <v>63</v>
+        <v>41</v>
       </c>
       <c r="H13" t="s">
         <v>45</v>
@@ -2166,7 +2163,7 @@
         <v>30</v>
       </c>
       <c r="G14" t="s">
-        <v>63</v>
+        <v>41</v>
       </c>
       <c r="H14" t="s">
         <v>45</v>
@@ -2186,7 +2183,7 @@
         <v>31</v>
       </c>
       <c r="G15" t="s">
-        <v>63</v>
+        <v>41</v>
       </c>
       <c r="H15" t="s">
         <v>45</v>
@@ -2286,7 +2283,7 @@
         <v>36</v>
       </c>
       <c r="G20" t="s">
-        <v>63</v>
+        <v>41</v>
       </c>
       <c r="H20" t="s">
         <v>45</v>
@@ -2363,7 +2360,7 @@
         <v>45</v>
       </c>
       <c r="F24" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G24" t="s">
         <v>41</v>
@@ -2434,23 +2431,23 @@
     </row>
     <row r="28" spans="1:13">
       <c r="F28" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="29" spans="1:13">
       <c r="F29" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="K29" t="s">
+        <v>64</v>
+      </c>
+      <c r="M29" t="s">
         <v>65</v>
-      </c>
-      <c r="M29" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="30" spans="1:13">
       <c r="F30" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>
@@ -2477,39 +2474,39 @@
         <v>20</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="18.75">
       <c r="A2" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="18.75">
       <c r="A3" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="18.75">
       <c r="A4" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="18.75">
       <c r="A5" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="18.75">
@@ -2517,47 +2514,47 @@
         <v>56</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="18.75">
       <c r="A7" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="18.75">
       <c r="A8" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="18.75">
       <c r="A9" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="18.75">
       <c r="A10" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="18.75">
       <c r="A11" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
   </sheetData>

</xml_diff>